<commit_message>
working on displaying times in xlsx
i'm dumb, didn't do times right, just saving progress
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -381,7 +381,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -395,7 +395,7 @@
         <v>Kitchen Open</v>
       </c>
       <c r="B1" t="str">
-        <v>josh Muma</v>
+        <v>fred york</v>
       </c>
     </row>
     <row r="2">
@@ -403,7 +403,7 @@
         <v>Kitchen Closed</v>
       </c>
       <c r="B2" t="str">
-        <v>Jordan</v>
+        <v>Emmie</v>
       </c>
     </row>
     <row r="3">
@@ -411,7 +411,7 @@
         <v>Production</v>
       </c>
       <c r="B3" t="str">
-        <v>josh Muma</v>
+        <v>flora</v>
       </c>
     </row>
     <row r="4">
@@ -419,7 +419,7 @@
         <v>Traditional Close</v>
       </c>
       <c r="B4" t="str">
-        <v>josh Muma</v>
+        <v>Jordan</v>
       </c>
     </row>
     <row r="5">
@@ -427,7 +427,7 @@
         <v>Sub Close</v>
       </c>
       <c r="B5" t="str">
-        <v>josh Muma</v>
+        <v>Jordan</v>
       </c>
     </row>
     <row r="6">
@@ -435,19 +435,35 @@
         <v>Traditional</v>
       </c>
       <c r="B6" t="str">
-        <v>josh Muma</v>
+        <v>Ruby</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v xml:space="preserve">Start time: </v>
+      </c>
+      <c r="B7">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v xml:space="preserve">End time: </v>
+      </c>
+      <c r="B8">
+        <v>1500</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B8"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -461,7 +477,7 @@
         <v>Kitchen Open</v>
       </c>
       <c r="B1" t="str">
-        <v>josh Muma</v>
+        <v>Emmie</v>
       </c>
     </row>
     <row r="2">
@@ -504,16 +520,32 @@
         <v>Emmie</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v xml:space="preserve">Start time: </v>
+      </c>
+      <c r="B7">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v xml:space="preserve">End time: </v>
+      </c>
+      <c r="B8">
+        <v>2200</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B8"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -526,29 +558,26 @@
       <c r="A1" t="str">
         <v>Kitchen Open</v>
       </c>
-      <c r="B1" t="str">
-        <v>josh Muma</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
         <v>Kitchen Closed</v>
       </c>
+      <c r="B2" t="str">
+        <v>Jordan</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
         <v>Production</v>
       </c>
-      <c r="B3" t="str">
-        <v>josh Muma</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
         <v>Traditional Close</v>
       </c>
       <c r="B4" t="str">
-        <v>Jordan</v>
+        <v>Ruby</v>
       </c>
     </row>
     <row r="5">
@@ -563,20 +592,33 @@
       <c r="A6" t="str">
         <v>Traditional</v>
       </c>
-      <c r="B6" t="str">
-        <v>josh Muma</v>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v xml:space="preserve">Start time: </v>
+      </c>
+      <c r="B7">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v xml:space="preserve">End time: </v>
+      </c>
+      <c r="B8">
+        <v>1500</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B8"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -606,7 +648,7 @@
         <v>Production</v>
       </c>
       <c r="B3" t="str">
-        <v>josh Muma</v>
+        <v>Emmie</v>
       </c>
     </row>
     <row r="4">
@@ -614,7 +656,7 @@
         <v>Traditional Close</v>
       </c>
       <c r="B4" t="str">
-        <v>josh Muma</v>
+        <v>Jordan</v>
       </c>
     </row>
     <row r="5">
@@ -622,7 +664,7 @@
         <v>Sub Close</v>
       </c>
       <c r="B5" t="str">
-        <v>josh Muma</v>
+        <v>Jordan</v>
       </c>
     </row>
     <row r="6">
@@ -633,16 +675,32 @@
         <v>Emmie</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v xml:space="preserve">Start time: </v>
+      </c>
+      <c r="B7">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v xml:space="preserve">End time: </v>
+      </c>
+      <c r="B8">
+        <v>2300</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B8"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -656,7 +714,7 @@
         <v>Kitchen Open</v>
       </c>
       <c r="B1" t="str">
-        <v>fred york</v>
+        <v>Emmie</v>
       </c>
     </row>
     <row r="2">
@@ -672,7 +730,7 @@
         <v>Production</v>
       </c>
       <c r="B3" t="str">
-        <v>fred york</v>
+        <v>Emmie</v>
       </c>
     </row>
     <row r="4">
@@ -699,16 +757,32 @@
         <v>Emmie</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v xml:space="preserve">Start time: </v>
+      </c>
+      <c r="B7">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v xml:space="preserve">End time: </v>
+      </c>
+      <c r="B8">
+        <v>2300</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B8"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -721,60 +795,58 @@
       <c r="A1" t="str">
         <v>Kitchen Open</v>
       </c>
-      <c r="B1" t="str">
-        <v>fred york</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
         <v>Kitchen Closed</v>
       </c>
-      <c r="B2" t="str">
-        <v>Jordan</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
         <v>Production</v>
       </c>
-      <c r="B3" t="str">
-        <v>fred york</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
         <v>Traditional Close</v>
       </c>
-      <c r="B4" t="str">
-        <v>josh Muma</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
         <v>Sub Close</v>
       </c>
-      <c r="B5" t="str">
-        <v>josh Muma</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
         <v>Traditional</v>
       </c>
-      <c r="B6" t="str">
-        <v>Emmie</v>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v xml:space="preserve">Start time: </v>
+      </c>
+      <c r="B7">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v xml:space="preserve">End time: </v>
+      </c>
+      <c r="B8">
+        <v>1400</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B8"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -787,53 +859,45 @@
       <c r="A1" t="str">
         <v>Kitchen Open</v>
       </c>
-      <c r="B1" t="str">
-        <v>fred york</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
         <v>Kitchen Closed</v>
       </c>
-      <c r="B2" t="str">
-        <v>flora</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
         <v>Production</v>
       </c>
-      <c r="B3" t="str">
-        <v>josh Muma</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
         <v>Traditional Close</v>
       </c>
-      <c r="B4" t="str">
-        <v>josh Muma</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
         <v>Sub Close</v>
       </c>
-      <c r="B5" t="str">
-        <v>josh Muma</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
         <v>Traditional</v>
       </c>
-      <c r="B6" t="str">
-        <v>Ruby</v>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v xml:space="preserve">Start time: </v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v xml:space="preserve">End time: </v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
working on showing the time for each skill
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -381,7 +381,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -392,78 +392,28 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Kitchen Open</v>
+        <v>Skill</v>
       </c>
       <c r="B1" t="str">
-        <v>fred york</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Kitchen Closed</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Emmie</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Production</v>
-      </c>
-      <c r="B3" t="str">
-        <v>flora</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Traditional Close</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Jordan</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Sub Close</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Jordan</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Traditional</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Ruby</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v xml:space="preserve">Start time: </v>
-      </c>
-      <c r="B7">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v xml:space="preserve">End time: </v>
-      </c>
-      <c r="B8">
-        <v>1500</v>
+        <v>Employee Name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Start Time</v>
+      </c>
+      <c r="D1" t="str">
+        <v>End Time</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -474,78 +424,28 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Kitchen Open</v>
+        <v>Skill</v>
       </c>
       <c r="B1" t="str">
-        <v>Emmie</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Kitchen Closed</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Ruby</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Production</v>
-      </c>
-      <c r="B3" t="str">
-        <v>flora</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Traditional Close</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Ruby</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Sub Close</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Ruby</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Traditional</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Emmie</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v xml:space="preserve">Start time: </v>
-      </c>
-      <c r="B7">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v xml:space="preserve">End time: </v>
-      </c>
-      <c r="B8">
-        <v>2200</v>
+        <v>Employee Name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Start Time</v>
+      </c>
+      <c r="D1" t="str">
+        <v>End Time</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -556,69 +456,28 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Kitchen Open</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Kitchen Closed</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Jordan</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Production</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Traditional Close</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Ruby</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Sub Close</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Jordan</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Traditional</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v xml:space="preserve">Start time: </v>
-      </c>
-      <c r="B7">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v xml:space="preserve">End time: </v>
-      </c>
-      <c r="B8">
-        <v>1500</v>
+        <v>Skill</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Employee Name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Start Time</v>
+      </c>
+      <c r="D1" t="str">
+        <v>End Time</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -629,78 +488,28 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Kitchen Open</v>
+        <v>Skill</v>
       </c>
       <c r="B1" t="str">
-        <v>Emmie</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Kitchen Closed</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Jordan</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Production</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Emmie</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Traditional Close</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Jordan</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Sub Close</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Jordan</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Traditional</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Emmie</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v xml:space="preserve">Start time: </v>
-      </c>
-      <c r="B7">
-        <v>1400</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v xml:space="preserve">End time: </v>
-      </c>
-      <c r="B8">
-        <v>2300</v>
+        <v>Employee Name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Start Time</v>
+      </c>
+      <c r="D1" t="str">
+        <v>End Time</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -711,78 +520,28 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Kitchen Open</v>
+        <v>Skill</v>
       </c>
       <c r="B1" t="str">
-        <v>Emmie</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Kitchen Closed</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Jordan</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Production</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Emmie</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Traditional Close</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Jordan</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Sub Close</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Jordan</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Traditional</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Emmie</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v xml:space="preserve">Start time: </v>
-      </c>
-      <c r="B7">
-        <v>1400</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v xml:space="preserve">End time: </v>
-      </c>
-      <c r="B8">
-        <v>2300</v>
+        <v>Employee Name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Start Time</v>
+      </c>
+      <c r="D1" t="str">
+        <v>End Time</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -793,60 +552,28 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Kitchen Open</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Kitchen Closed</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Production</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Traditional Close</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Sub Close</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Traditional</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v xml:space="preserve">Start time: </v>
-      </c>
-      <c r="B7">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v xml:space="preserve">End time: </v>
-      </c>
-      <c r="B8">
-        <v>1400</v>
+        <v>Skill</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Employee Name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Start Time</v>
+      </c>
+      <c r="D1" t="str">
+        <v>End Time</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -857,47 +584,21 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Kitchen Open</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Kitchen Closed</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Production</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Traditional Close</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Sub Close</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Traditional</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v xml:space="preserve">Start time: </v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v xml:space="preserve">End time: </v>
+        <v>Skill</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Employee Name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Start Time</v>
+      </c>
+      <c r="D1" t="str">
+        <v>End Time</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>